<commit_message>
Updated to estimated selectivity - having convergence issues though
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_230111.xlsx
+++ b/data/hake_intrasp_230111.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EC942D-7B1C-C046-AF34-0DEDD414EF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46E8E8D-41F0-6D41-90C4-10C359507D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8620" yWindow="5860" windowWidth="45360" windowHeight="32740" firstSheet="9" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6980" yWindow="500" windowWidth="26620" windowHeight="20500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">UobsWtAge!$A$1:$I$166</definedName>
+    <definedName name="DiagnosticTables" localSheetId="2">fleet_control!$H$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1908,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="B28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12477,7 +12478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="S36" sqref="S36"/>
     </sheetView>
   </sheetViews>
@@ -17189,7 +17190,7 @@
   <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17200,6 +17201,7 @@
     <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -17302,7 +17304,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G2">
         <v>6</v>
@@ -17361,7 +17363,7 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G3">
         <v>6</v>
@@ -18199,15 +18201,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -18233,7 +18238,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>473</v>
       </c>
@@ -18258,8 +18263,9 @@
       <c r="H2">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>473</v>
       </c>
@@ -18284,8 +18290,9 @@
       <c r="H3">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>473</v>
       </c>
@@ -18310,8 +18317,9 @@
       <c r="H4">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>473</v>
       </c>
@@ -18336,8 +18344,9 @@
       <c r="H5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>473</v>
       </c>
@@ -18362,8 +18371,9 @@
       <c r="H6">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>473</v>
       </c>
@@ -18388,8 +18398,9 @@
       <c r="H7">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>473</v>
       </c>
@@ -18414,8 +18425,9 @@
       <c r="H8">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>473</v>
       </c>
@@ -18440,8 +18452,9 @@
       <c r="H9">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>473</v>
       </c>
@@ -18466,8 +18479,9 @@
       <c r="H10">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>473</v>
       </c>
@@ -18492,8 +18506,9 @@
       <c r="H11">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>473</v>
       </c>
@@ -18518,8 +18533,9 @@
       <c r="H12">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>473</v>
       </c>
@@ -18544,8 +18560,9 @@
       <c r="H13">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>473</v>
       </c>
@@ -18570,8 +18587,9 @@
       <c r="H14">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>473</v>
       </c>
@@ -18596,8 +18614,9 @@
       <c r="H15">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>473</v>
       </c>
@@ -18622,8 +18641,9 @@
       <c r="H16">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>473</v>
       </c>
@@ -18648,8 +18668,9 @@
       <c r="H17">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>473</v>
       </c>
@@ -18674,8 +18695,9 @@
       <c r="H18">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>473</v>
       </c>
@@ -18700,8 +18722,9 @@
       <c r="H19">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>473</v>
       </c>
@@ -18726,8 +18749,9 @@
       <c r="H20">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>473</v>
       </c>
@@ -18752,8 +18776,9 @@
       <c r="H21">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>473</v>
       </c>
@@ -18778,8 +18803,9 @@
       <c r="H22">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>473</v>
       </c>
@@ -18804,8 +18830,9 @@
       <c r="H23">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>473</v>
       </c>
@@ -18830,8 +18857,9 @@
       <c r="H24">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>473</v>
       </c>
@@ -18856,8 +18884,9 @@
       <c r="H25">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>473</v>
       </c>
@@ -18882,8 +18911,9 @@
       <c r="H26">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>473</v>
       </c>
@@ -18908,8 +18938,9 @@
       <c r="H27">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>473</v>
       </c>
@@ -18934,8 +18965,9 @@
       <c r="H28">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>473</v>
       </c>
@@ -18960,8 +18992,9 @@
       <c r="H29">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>473</v>
       </c>
@@ -18986,8 +19019,9 @@
       <c r="H30">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>473</v>
       </c>
@@ -19012,8 +19046,9 @@
       <c r="H31">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>473</v>
       </c>
@@ -19038,8 +19073,9 @@
       <c r="H32">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>473</v>
       </c>
@@ -19064,8 +19100,9 @@
       <c r="H33">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>473</v>
       </c>
@@ -19090,8 +19127,9 @@
       <c r="H34">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>473</v>
       </c>
@@ -19116,8 +19154,9 @@
       <c r="H35">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>473</v>
       </c>
@@ -19142,8 +19181,9 @@
       <c r="H36">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>473</v>
       </c>
@@ -19168,8 +19208,9 @@
       <c r="H37">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>473</v>
       </c>
@@ -19194,8 +19235,9 @@
       <c r="H38">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>473</v>
       </c>
@@ -19220,8 +19262,9 @@
       <c r="H39">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>473</v>
       </c>
@@ -19246,8 +19289,9 @@
       <c r="H40">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>473</v>
       </c>
@@ -19272,6 +19316,7 @@
       <c r="H41">
         <v>0.01</v>
       </c>
+      <c r="I41" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23446,8 +23491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Y81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:Y1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Now using correct number of ages in selectivity estimation
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_230111.xlsx
+++ b/data/hake_intrasp_230111.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46E8E8D-41F0-6D41-90C4-10C359507D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353710E6-3F56-0549-AF18-FBADC985CCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6980" yWindow="500" windowWidth="26620" windowHeight="20500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6980" yWindow="500" windowWidth="26620" windowHeight="20500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -1909,7 +1909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -17189,12 +17189,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
@@ -17307,7 +17308,7 @@
         <v>5</v>
       </c>
       <c r="G2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -17366,7 +17367,7 @@
         <v>5</v>
       </c>
       <c r="G3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -23491,7 +23492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Y81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated survey catchability to match assessment
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_230111.xlsx
+++ b/data/hake_intrasp_230111.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353710E6-3F56-0549-AF18-FBADC985CCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AF4FCE-0F94-0D40-9A75-F48F024D932F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6980" yWindow="500" windowWidth="26620" windowHeight="20500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="42700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -1909,7 +1909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -17190,19 +17190,38 @@
   <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -17397,19 +17416,16 @@
         <v>1</v>
       </c>
       <c r="Q3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
         <v>0</v>
-      </c>
-      <c r="U3">
-        <v>0.01</v>
       </c>
       <c r="V3">
         <v>0</v>

</xml_diff>

<commit_message>
Added a switch to the code for keeping M1 = 0.21
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_230111.xlsx
+++ b/data/hake_intrasp_230111.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AF4FCE-0F94-0D40-9A75-F48F024D932F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA359757-635D-284F-8866-4A71091190B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="42700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -1909,7 +1909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -11702,7 +11702,7 @@
   <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:Q2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14789,8 +14789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView zoomScale="175" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17189,7 +17189,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Attempted an age-variant update of M1. Doesn't appear to work.
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_230111.xlsx
+++ b/data/hake_intrasp_230111.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA359757-635D-284F-8866-4A71091190B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D484F7B-65E2-D044-8938-A48A1B904319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -3859,8 +3859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:T121"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3941,7 +3941,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>1980</v>
@@ -4003,7 +4003,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>1981</v>
@@ -4065,7 +4065,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>1982</v>
@@ -4127,7 +4127,7 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>1983</v>
@@ -4189,7 +4189,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>1984</v>
@@ -4251,7 +4251,7 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>1985</v>
@@ -4313,7 +4313,7 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>1986</v>
@@ -4375,7 +4375,7 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>1987</v>
@@ -4437,7 +4437,7 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>1988</v>
@@ -4499,7 +4499,7 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>1989</v>
@@ -4561,7 +4561,7 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>1990</v>
@@ -4623,7 +4623,7 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
         <v>1991</v>
@@ -4685,7 +4685,7 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>1992</v>
@@ -4747,7 +4747,7 @@
         <v>1</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15">
         <v>1993</v>
@@ -4809,7 +4809,7 @@
         <v>1</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <v>1994</v>
@@ -4871,7 +4871,7 @@
         <v>1</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
         <v>1995</v>
@@ -4933,7 +4933,7 @@
         <v>1</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <v>1996</v>
@@ -4995,7 +4995,7 @@
         <v>1</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <v>1997</v>
@@ -5057,7 +5057,7 @@
         <v>1</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20">
         <v>1998</v>
@@ -5119,7 +5119,7 @@
         <v>1</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <v>1999</v>
@@ -5181,7 +5181,7 @@
         <v>1</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <v>2000</v>
@@ -5243,7 +5243,7 @@
         <v>1</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <v>2001</v>
@@ -5305,7 +5305,7 @@
         <v>1</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <v>2002</v>
@@ -5367,7 +5367,7 @@
         <v>1</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>2003</v>
@@ -5429,7 +5429,7 @@
         <v>1</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26">
         <v>2004</v>
@@ -5491,7 +5491,7 @@
         <v>1</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27">
         <v>2005</v>
@@ -5553,7 +5553,7 @@
         <v>1</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28">
         <v>2006</v>
@@ -5615,7 +5615,7 @@
         <v>1</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29">
         <v>2007</v>
@@ -5677,7 +5677,7 @@
         <v>1</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30">
         <v>2008</v>
@@ -5739,7 +5739,7 @@
         <v>1</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31">
         <v>2009</v>
@@ -5801,7 +5801,7 @@
         <v>1</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32">
         <v>2010</v>
@@ -5863,7 +5863,7 @@
         <v>1</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33">
         <v>2011</v>
@@ -5925,7 +5925,7 @@
         <v>1</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34">
         <v>2012</v>
@@ -5987,7 +5987,7 @@
         <v>1</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35">
         <v>2013</v>
@@ -6049,7 +6049,7 @@
         <v>1</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36">
         <v>2014</v>
@@ -6111,7 +6111,7 @@
         <v>1</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37">
         <v>2015</v>
@@ -6173,7 +6173,7 @@
         <v>1</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38">
         <v>2016</v>
@@ -6235,7 +6235,7 @@
         <v>1</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39">
         <v>2017</v>
@@ -6297,7 +6297,7 @@
         <v>1</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E40">
         <v>2018</v>
@@ -6359,7 +6359,7 @@
         <v>1</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41">
         <v>2019</v>
@@ -6421,7 +6421,7 @@
         <v>1</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42">
         <v>1980</v>
@@ -6483,7 +6483,7 @@
         <v>1</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43">
         <v>1981</v>
@@ -6545,7 +6545,7 @@
         <v>1</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44">
         <v>1982</v>
@@ -6607,7 +6607,7 @@
         <v>1</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45">
         <v>1983</v>
@@ -6669,7 +6669,7 @@
         <v>1</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46">
         <v>1984</v>
@@ -6731,7 +6731,7 @@
         <v>1</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47">
         <v>1985</v>
@@ -6793,7 +6793,7 @@
         <v>1</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48">
         <v>1986</v>
@@ -6855,7 +6855,7 @@
         <v>1</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E49">
         <v>1987</v>
@@ -6917,7 +6917,7 @@
         <v>1</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50">
         <v>1988</v>
@@ -6979,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51">
         <v>1989</v>
@@ -7041,7 +7041,7 @@
         <v>1</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E52">
         <v>1990</v>
@@ -7103,7 +7103,7 @@
         <v>1</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E53">
         <v>1991</v>
@@ -7165,7 +7165,7 @@
         <v>1</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54">
         <v>1992</v>
@@ -7227,7 +7227,7 @@
         <v>1</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E55">
         <v>1993</v>
@@ -7289,7 +7289,7 @@
         <v>1</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E56">
         <v>1994</v>
@@ -7351,7 +7351,7 @@
         <v>1</v>
       </c>
       <c r="D57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57">
         <v>1995</v>
@@ -7413,7 +7413,7 @@
         <v>1</v>
       </c>
       <c r="D58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E58">
         <v>1996</v>
@@ -7475,7 +7475,7 @@
         <v>1</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E59">
         <v>1997</v>
@@ -7537,7 +7537,7 @@
         <v>1</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60">
         <v>1998</v>
@@ -7599,7 +7599,7 @@
         <v>1</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E61">
         <v>1999</v>
@@ -7661,7 +7661,7 @@
         <v>1</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E62">
         <v>2000</v>
@@ -7723,7 +7723,7 @@
         <v>1</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E63">
         <v>2001</v>
@@ -7785,7 +7785,7 @@
         <v>1</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E64">
         <v>2002</v>
@@ -7847,7 +7847,7 @@
         <v>1</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E65">
         <v>2003</v>
@@ -7909,7 +7909,7 @@
         <v>1</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E66">
         <v>2004</v>
@@ -7971,7 +7971,7 @@
         <v>1</v>
       </c>
       <c r="D67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E67">
         <v>2005</v>
@@ -8033,7 +8033,7 @@
         <v>1</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E68">
         <v>2006</v>
@@ -8095,7 +8095,7 @@
         <v>1</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E69">
         <v>2007</v>
@@ -8157,7 +8157,7 @@
         <v>1</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70">
         <v>2008</v>
@@ -8219,7 +8219,7 @@
         <v>1</v>
       </c>
       <c r="D71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E71">
         <v>2009</v>
@@ -8281,7 +8281,7 @@
         <v>1</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E72">
         <v>2010</v>
@@ -8343,7 +8343,7 @@
         <v>1</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E73">
         <v>2011</v>
@@ -8405,7 +8405,7 @@
         <v>1</v>
       </c>
       <c r="D74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E74">
         <v>2012</v>
@@ -8467,7 +8467,7 @@
         <v>1</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E75">
         <v>2013</v>
@@ -8529,7 +8529,7 @@
         <v>1</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E76">
         <v>2014</v>
@@ -8591,7 +8591,7 @@
         <v>1</v>
       </c>
       <c r="D77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E77">
         <v>2015</v>
@@ -8653,7 +8653,7 @@
         <v>1</v>
       </c>
       <c r="D78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E78">
         <v>2016</v>
@@ -8715,7 +8715,7 @@
         <v>1</v>
       </c>
       <c r="D79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E79">
         <v>2017</v>
@@ -8777,7 +8777,7 @@
         <v>1</v>
       </c>
       <c r="D80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E80">
         <v>2018</v>
@@ -8839,7 +8839,7 @@
         <v>1</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E81">
         <v>2019</v>
@@ -8901,7 +8901,7 @@
         <v>1</v>
       </c>
       <c r="D82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E82">
         <v>1980</v>
@@ -8963,7 +8963,7 @@
         <v>1</v>
       </c>
       <c r="D83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E83">
         <v>1981</v>
@@ -9025,7 +9025,7 @@
         <v>1</v>
       </c>
       <c r="D84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E84">
         <v>1982</v>
@@ -9087,7 +9087,7 @@
         <v>1</v>
       </c>
       <c r="D85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E85">
         <v>1983</v>
@@ -9149,7 +9149,7 @@
         <v>1</v>
       </c>
       <c r="D86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E86">
         <v>1984</v>
@@ -9211,7 +9211,7 @@
         <v>1</v>
       </c>
       <c r="D87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E87">
         <v>1985</v>
@@ -9273,7 +9273,7 @@
         <v>1</v>
       </c>
       <c r="D88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E88">
         <v>1986</v>
@@ -9335,7 +9335,7 @@
         <v>1</v>
       </c>
       <c r="D89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E89">
         <v>1987</v>
@@ -9397,7 +9397,7 @@
         <v>1</v>
       </c>
       <c r="D90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E90">
         <v>1988</v>
@@ -9459,7 +9459,7 @@
         <v>1</v>
       </c>
       <c r="D91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E91">
         <v>1989</v>
@@ -9521,7 +9521,7 @@
         <v>1</v>
       </c>
       <c r="D92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E92">
         <v>1990</v>
@@ -9583,7 +9583,7 @@
         <v>1</v>
       </c>
       <c r="D93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E93">
         <v>1991</v>
@@ -9645,7 +9645,7 @@
         <v>1</v>
       </c>
       <c r="D94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E94">
         <v>1992</v>
@@ -9707,7 +9707,7 @@
         <v>1</v>
       </c>
       <c r="D95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E95">
         <v>1993</v>
@@ -9769,7 +9769,7 @@
         <v>1</v>
       </c>
       <c r="D96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96">
         <v>1994</v>
@@ -9831,7 +9831,7 @@
         <v>1</v>
       </c>
       <c r="D97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E97">
         <v>1995</v>
@@ -9893,7 +9893,7 @@
         <v>1</v>
       </c>
       <c r="D98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E98">
         <v>1996</v>
@@ -9955,7 +9955,7 @@
         <v>1</v>
       </c>
       <c r="D99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99">
         <v>1997</v>
@@ -10017,7 +10017,7 @@
         <v>1</v>
       </c>
       <c r="D100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E100">
         <v>1998</v>
@@ -10079,7 +10079,7 @@
         <v>1</v>
       </c>
       <c r="D101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E101">
         <v>1999</v>
@@ -10141,7 +10141,7 @@
         <v>1</v>
       </c>
       <c r="D102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102">
         <v>2000</v>
@@ -10203,7 +10203,7 @@
         <v>1</v>
       </c>
       <c r="D103">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E103">
         <v>2001</v>
@@ -10265,7 +10265,7 @@
         <v>1</v>
       </c>
       <c r="D104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E104">
         <v>2002</v>
@@ -10327,7 +10327,7 @@
         <v>1</v>
       </c>
       <c r="D105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E105">
         <v>2003</v>
@@ -10389,7 +10389,7 @@
         <v>1</v>
       </c>
       <c r="D106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E106">
         <v>2004</v>
@@ -10451,7 +10451,7 @@
         <v>1</v>
       </c>
       <c r="D107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E107">
         <v>2005</v>
@@ -10513,7 +10513,7 @@
         <v>1</v>
       </c>
       <c r="D108">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E108">
         <v>2006</v>
@@ -10575,7 +10575,7 @@
         <v>1</v>
       </c>
       <c r="D109">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E109">
         <v>2007</v>
@@ -10637,7 +10637,7 @@
         <v>1</v>
       </c>
       <c r="D110">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E110">
         <v>2008</v>
@@ -10699,7 +10699,7 @@
         <v>1</v>
       </c>
       <c r="D111">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E111">
         <v>2009</v>
@@ -10761,7 +10761,7 @@
         <v>1</v>
       </c>
       <c r="D112">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E112">
         <v>2010</v>
@@ -10823,7 +10823,7 @@
         <v>1</v>
       </c>
       <c r="D113">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E113">
         <v>2011</v>
@@ -10885,7 +10885,7 @@
         <v>1</v>
       </c>
       <c r="D114">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E114">
         <v>2012</v>
@@ -10947,7 +10947,7 @@
         <v>1</v>
       </c>
       <c r="D115">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E115">
         <v>2013</v>
@@ -11009,7 +11009,7 @@
         <v>1</v>
       </c>
       <c r="D116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E116">
         <v>2014</v>
@@ -11071,7 +11071,7 @@
         <v>1</v>
       </c>
       <c r="D117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E117">
         <v>2015</v>
@@ -11133,7 +11133,7 @@
         <v>1</v>
       </c>
       <c r="D118">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E118">
         <v>2016</v>
@@ -11195,7 +11195,7 @@
         <v>1</v>
       </c>
       <c r="D119">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E119">
         <v>2017</v>
@@ -11257,7 +11257,7 @@
         <v>1</v>
       </c>
       <c r="D120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E120">
         <v>2018</v>
@@ -11319,7 +11319,7 @@
         <v>1</v>
       </c>
       <c r="D121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E121">
         <v>2019</v>
@@ -14789,8 +14789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScale="175" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Attempting to generalize code to work for any year range. Not working.
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_230111.xlsx
+++ b/data/hake_intrasp_230111.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D484F7B-65E2-D044-8938-A48A1B904319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DC2E63-B330-7646-9D4A-91BD96282B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -1909,7 +1909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -3859,7 +3859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:T121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D121"/>
     </sheetView>
   </sheetViews>
@@ -14789,8 +14789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView zoomScale="175" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>